<commit_message>
stop the train correctly red line
</commit_message>
<xml_diff>
--- a/resources/Red Line.xlsx
+++ b/resources/Red Line.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/07de44e608f1ac43/Documents/GitHub/ECE1140-Project/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{72CF944D-3F9F-4499-94C3-63703778A7E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{517A005F-F11A-4994-A256-7C5A1832339A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -657,9 +657,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G62" sqref="G62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -669,7 +669,7 @@
     <col min="3" max="3" width="8.453125" style="3" customWidth="1"/>
     <col min="4" max="4" width="22.26953125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.26953125" style="3" customWidth="1"/>
-    <col min="6" max="7" width="33.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="39.36328125" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" style="3" customWidth="1"/>
     <col min="9" max="9" width="10.54296875" style="3" customWidth="1"/>
     <col min="10" max="11" width="13.26953125" style="3" customWidth="1"/>
@@ -956,6 +956,12 @@
       <c r="D8" s="3" t="s">
         <v>31</v>
       </c>
+      <c r="E8" s="3">
+        <v>0</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>60</v>
+      </c>
       <c r="H8" s="3">
         <v>75</v>
       </c>
@@ -992,12 +998,6 @@
       <c r="C9" s="3">
         <v>8</v>
       </c>
-      <c r="E9" s="3">
-        <v>0</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>60</v>
-      </c>
       <c r="H9" s="3">
         <v>75</v>
       </c>
@@ -1450,6 +1450,12 @@
       <c r="D22" s="3" t="s">
         <v>33</v>
       </c>
+      <c r="E22" s="3">
+        <v>1</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>62</v>
+      </c>
       <c r="H22" s="3">
         <v>100</v>
       </c>
@@ -1486,12 +1492,6 @@
       <c r="C23" s="5">
         <v>22</v>
       </c>
-      <c r="E23" s="3">
-        <v>1</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="H23" s="3">
         <v>100</v>
       </c>
@@ -2360,6 +2360,12 @@
       <c r="D46" s="3" t="s">
         <v>36</v>
       </c>
+      <c r="E46" s="3">
+        <v>1</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>58</v>
+      </c>
       <c r="H46" s="3">
         <v>50</v>
       </c>
@@ -2398,12 +2404,6 @@
       <c r="C47" s="3">
         <v>46</v>
       </c>
-      <c r="E47" s="3">
-        <v>1</v>
-      </c>
-      <c r="G47" s="3" t="s">
-        <v>58</v>
-      </c>
       <c r="H47" s="3">
         <v>75</v>
       </c>
@@ -2439,12 +2439,6 @@
       <c r="C48" s="5">
         <v>47</v>
       </c>
-      <c r="E48" s="3">
-        <v>0</v>
-      </c>
-      <c r="F48" s="3" t="s">
-        <v>59</v>
-      </c>
       <c r="H48" s="3">
         <v>75</v>
       </c>
@@ -2482,6 +2476,12 @@
       </c>
       <c r="D49" s="3" t="s">
         <v>37</v>
+      </c>
+      <c r="E49" s="3">
+        <v>0</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="H49" s="3">
         <v>75</v>

</xml_diff>

<commit_message>
stop the train correctly red line (#320)
</commit_message>
<xml_diff>
--- a/resources/Red Line.xlsx
+++ b/resources/Red Line.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/07de44e608f1ac43/Documents/GitHub/ECE1140-Project/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{72CF944D-3F9F-4499-94C3-63703778A7E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{517A005F-F11A-4994-A256-7C5A1832339A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -657,9 +657,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G62" sqref="G62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -669,7 +669,7 @@
     <col min="3" max="3" width="8.453125" style="3" customWidth="1"/>
     <col min="4" max="4" width="22.26953125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.26953125" style="3" customWidth="1"/>
-    <col min="6" max="7" width="33.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="39.36328125" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" style="3" customWidth="1"/>
     <col min="9" max="9" width="10.54296875" style="3" customWidth="1"/>
     <col min="10" max="11" width="13.26953125" style="3" customWidth="1"/>
@@ -956,6 +956,12 @@
       <c r="D8" s="3" t="s">
         <v>31</v>
       </c>
+      <c r="E8" s="3">
+        <v>0</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>60</v>
+      </c>
       <c r="H8" s="3">
         <v>75</v>
       </c>
@@ -992,12 +998,6 @@
       <c r="C9" s="3">
         <v>8</v>
       </c>
-      <c r="E9" s="3">
-        <v>0</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>60</v>
-      </c>
       <c r="H9" s="3">
         <v>75</v>
       </c>
@@ -1450,6 +1450,12 @@
       <c r="D22" s="3" t="s">
         <v>33</v>
       </c>
+      <c r="E22" s="3">
+        <v>1</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>62</v>
+      </c>
       <c r="H22" s="3">
         <v>100</v>
       </c>
@@ -1486,12 +1492,6 @@
       <c r="C23" s="5">
         <v>22</v>
       </c>
-      <c r="E23" s="3">
-        <v>1</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="H23" s="3">
         <v>100</v>
       </c>
@@ -2360,6 +2360,12 @@
       <c r="D46" s="3" t="s">
         <v>36</v>
       </c>
+      <c r="E46" s="3">
+        <v>1</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>58</v>
+      </c>
       <c r="H46" s="3">
         <v>50</v>
       </c>
@@ -2398,12 +2404,6 @@
       <c r="C47" s="3">
         <v>46</v>
       </c>
-      <c r="E47" s="3">
-        <v>1</v>
-      </c>
-      <c r="G47" s="3" t="s">
-        <v>58</v>
-      </c>
       <c r="H47" s="3">
         <v>75</v>
       </c>
@@ -2439,12 +2439,6 @@
       <c r="C48" s="5">
         <v>47</v>
       </c>
-      <c r="E48" s="3">
-        <v>0</v>
-      </c>
-      <c r="F48" s="3" t="s">
-        <v>59</v>
-      </c>
       <c r="H48" s="3">
         <v>75</v>
       </c>
@@ -2482,6 +2476,12 @@
       </c>
       <c r="D49" s="3" t="s">
         <v>37</v>
+      </c>
+      <c r="E49" s="3">
+        <v>0</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="H49" s="3">
         <v>75</v>

</xml_diff>